<commit_message>
The Daily News Digest Bot
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\revan\Videos\N8N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D41770-0EC1-49CD-99C2-22C9885DEC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49FED84-77C8-47BA-A273-425A67C7B8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A8EF771E-6C41-48FA-8835-29E1B749273C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>FormMail.json</t>
+  </si>
+  <si>
+    <t>The Daily News Digest Bot</t>
+  </si>
+  <si>
+    <t>The Daily News Digest Bot.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this workflow automates the entire process of news using  telegram scheduled timing and triggered message </t>
   </si>
 </sst>
 </file>
@@ -464,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3405AF90-70F3-455C-B515-1EE882459FC6}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,6 +543,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45898</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
day 10 of n8n
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\revan\Videos\N8N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBDA261-616E-4115-9E4C-E82A9D7F68C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B3775D-B375-4351-AA12-A709C10A5561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A8EF771E-6C41-48FA-8835-29E1B749273C}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" xr2:uid="{A8EF771E-6C41-48FA-8835-29E1B749273C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Workshop Automation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this workflow is designed to send event registration and other event related things automatically </t>
+  </si>
+  <si>
+    <t>Workshop.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated Shop invoice </t>
   </si>
 </sst>
 </file>
@@ -485,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3405AF90-70F3-455C-B515-1EE882459FC6}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,6 +613,37 @@
       <c r="A8" s="1">
         <v>45900</v>
       </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>45901</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>